<commit_message>
Added functions for mask based analyses in segmenty by schedule.
</commit_message>
<xml_diff>
--- a/Data/P0/P0_HairCells_SegSchedule.xlsx
+++ b/Data/P0/P0_HairCells_SegSchedule.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PC\Box Sync\Research\Projects\Vestibular Hair Cell Analysis\Ear-Cell-Analysis-Code\Data\P0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E7FBB65-E82B-4017-B557-CE45CCE8638E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A688C95D-4982-46DB-85E8-FD07E4A5ED63}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="34395" yWindow="0" windowWidth="17205" windowHeight="21000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="16485" yWindow="90" windowWidth="17205" windowHeight="21000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -51,9 +51,6 @@
     <t>flatfield</t>
   </si>
   <si>
-    <t>threshold</t>
-  </si>
-  <si>
     <t>close</t>
   </si>
   <si>
@@ -70,6 +67,9 @@
   </si>
   <si>
     <t>gt</t>
+  </si>
+  <si>
+    <t>binarize</t>
   </si>
 </sst>
 </file>
@@ -390,10 +390,14 @@
   <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+      <selection activeCell="E13" sqref="E12:E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.140625" customWidth="1"/>
+    <col min="2" max="2" width="20.7109375" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -451,7 +455,7 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="B7">
         <v>0.2</v>
@@ -459,7 +463,7 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B8">
         <v>3</v>
@@ -467,7 +471,7 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B9">
         <v>6</v>
@@ -475,7 +479,7 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B10">
         <v>2</v>
@@ -483,12 +487,12 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B12">
         <v>1</v>
@@ -497,7 +501,7 @@
         <v>5</v>
       </c>
       <c r="D12" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E12">
         <v>20</v>

</xml_diff>